<commit_message>
Testando comandos MySQL Curso 2 Semana 8
</commit_message>
<xml_diff>
--- a/Week_8/Curso2/Aula4.1SQL/PRODUTOS.xlsx
+++ b/Week_8/Curso2/Aula4.1SQL/PRODUTOS.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="11_08BCD87B106D20C81D4B4620F92655EBDAFCF993" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{070ABEB7-9130-4791-B862-95DE42C2E493}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -506,7 +506,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>